<commit_message>
Upload updated booked hours for Week 2
</commit_message>
<xml_diff>
--- a/Organisational/Members/Truong/Booked_Hours_Truong.xlsx
+++ b/Organisational/Members/Truong/Booked_Hours_Truong.xlsx
@@ -1,28 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelw/CSSE/CITS3200/Administrivia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truon\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{31A31D98-CA30-574B-8C94-F50C456CB544}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8A31E6-55C5-444C-98F1-3BD43FEF2B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="21780" windowHeight="15340" tabRatio="500"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BookedHours" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
   <si>
     <t>Wk</t>
   </si>
@@ -50,8 +63,17 @@
 Hours</t>
   </si>
   <si>
+    <t>29/07/2025</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>Group meeting</t>
+  </si>
+  <si>
     <r>
-      <t>CITS3200 Project Billed Hours Record for &lt;YOUR NAME GOES HERE&gt;</t>
+      <t>CITS3200 Project Billed Hours Record for Xuan Truong Nguyen</t>
     </r>
     <r>
       <rPr>
@@ -59,16 +81,15 @@
         <rFont val="Lucida Sans"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">
-Each time you do some work on the project, note the week number, start and end date and hour, plus a brief description of the activity. At the end of each week send a copy of the sheet as it currently stands to your group's manager for recording on the group TimeSheet. Date in the form DD/MM/YY and time as XX:YY (24hr clock)</t>
+      <t xml:space="preserve"> and end date and hour, plus a brief description of the activity. At the end of each week send a copy of the sheet as it currently stands to your group's manager for recording on the group TimeSheet. Date in the form DD/MM/YY and time as XX:YY (24hr clock)</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -281,23 +302,15 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -321,7 +334,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -735,63 +756,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I65536"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.64453125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="46.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="1"/>
-    <col min="9" max="9" width="10.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="1" width="5.8203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.3515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.17578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.8203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="46.46875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.3515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.64453125" style="1"/>
+    <col min="9" max="9" width="10.64453125" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.64453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="71" customHeight="1">
-      <c r="A1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" ht="16" customHeight="1">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
+    <row r="1" spans="1:9" ht="71" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="13" customHeight="1">
-      <c r="A3" s="8"/>
+    <row r="3" spans="1:9" ht="13.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -805,46 +826,60 @@
         <v>3</v>
       </c>
       <c r="F3" s="18"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
-      <c r="G4" s="6" t="str">
-        <f>IF(I4&gt;0,I4,IF(I4=0, " ", "ERROR"))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H4" s="1" t="str">
-        <f>IF(G4&lt;&gt;"ERROR",G4)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I4" s="1">
+      <c r="G3" s="9"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="I4" s="1" t="e">
         <f>((D4+E4)-(B4+C4))*24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
-      <c r="G5" s="6" t="str">
+      <c r="G5" s="6" t="e">
         <f t="shared" ref="G5:G30" si="0">IF(I5&gt;0,I5,IF(I5=0, " ", "ERROR"))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H5" s="1" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H5" s="1" t="e">
         <f>IF(AND(G5&lt;&gt;" ",G5&lt;&gt;"ERROR",H4&lt;&gt;" ", H4&lt;&gt;"ERROR"),G5+H4," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I5" s="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I5" s="1" t="e">
         <f t="shared" ref="I5:I68" si="1">((D5+E5)-(B5+C5))*24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
@@ -853,16 +888,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H6" s="1" t="str">
+      <c r="H6" s="1" t="e">
         <f t="shared" ref="H6:H30" si="2">IF(AND(G6&lt;&gt;" ",G6&lt;&gt;"ERROR",H5&lt;&gt;" ", H5&lt;&gt;"ERROR"),G6+H5," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
@@ -871,16 +906,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H7" s="1" t="str">
+      <c r="H7" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="4"/>
@@ -889,16 +924,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H8" s="1" t="str">
+      <c r="H8" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
@@ -907,16 +942,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H9" s="1" t="str">
+      <c r="H9" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="4"/>
@@ -925,16 +960,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H10" s="1" t="str">
+      <c r="H10" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="4"/>
@@ -943,16 +978,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H11" s="1" t="str">
+      <c r="H11" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="4"/>
@@ -961,16 +996,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H12" s="1" t="str">
+      <c r="H12" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
@@ -979,16 +1014,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H13" s="1" t="str">
+      <c r="H13" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="4"/>
@@ -997,16 +1032,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H14" s="1" t="str">
+      <c r="H14" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="4"/>
@@ -1015,16 +1050,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H15" s="1" t="str">
+      <c r="H15" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="4"/>
@@ -1033,16 +1068,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H16" s="1" t="str">
+      <c r="H16" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="4"/>
@@ -1051,16 +1086,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H17" s="1" t="str">
+      <c r="H17" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="4"/>
@@ -1069,16 +1104,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H18" s="1" t="str">
+      <c r="H18" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
@@ -1087,16 +1122,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H19" s="1" t="str">
+      <c r="H19" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="4"/>
@@ -1105,16 +1140,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H20" s="1" t="str">
+      <c r="H20" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="4"/>
@@ -1123,16 +1158,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H21" s="1" t="str">
+      <c r="H21" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="4"/>
@@ -1141,16 +1176,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H22" s="1" t="str">
+      <c r="H22" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="4"/>
@@ -1159,16 +1194,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H23" s="1" t="str">
+      <c r="H23" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="4"/>
@@ -1177,16 +1212,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H24" s="1" t="str">
+      <c r="H24" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="4"/>
@@ -1195,16 +1230,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H25" s="1" t="str">
+      <c r="H25" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="4"/>
@@ -1213,16 +1248,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H26" s="1" t="str">
+      <c r="H26" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="4"/>
@@ -1231,16 +1266,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H27" s="1" t="str">
+      <c r="H27" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="4"/>
@@ -1249,16 +1284,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H28" s="1" t="str">
+      <c r="H28" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I28" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
       <c r="D29" s="4"/>
@@ -1267,16 +1302,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H29" s="1" t="str">
+      <c r="H29" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I29" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="4"/>
@@ -1285,34 +1320,34 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H30" s="1" t="str">
+      <c r="H30" s="1" t="e">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="16">
-      <c r="A31" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="9" t="s">
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.4">
+      <c r="A31" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="9" t="s">
+      <c r="C31" s="16"/>
+      <c r="D31" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="11" t="s">
+      <c r="E31" s="16"/>
+      <c r="F31" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I31" s="1" t="e">
@@ -1320,8 +1355,8 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="16">
-      <c r="A32" s="8"/>
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.4">
+      <c r="A32" s="9"/>
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
@@ -1334,15 +1369,15 @@
       <c r="E32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
       <c r="I32" s="1" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="4"/>
@@ -1351,16 +1386,16 @@
         <f t="shared" ref="G33:G64" si="3">IF(I33&gt;0,I33,IF(I33=0, " ", "ERROR"))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H33" s="1" t="str">
+      <c r="H33" s="1" t="e">
         <f>IF(AND(G33&lt;&gt;" ",G33&lt;&gt;"ERROR",H30&lt;&gt;" ", H30&lt;&gt;"ERROR"),G33+H30," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I33" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
       <c r="D34" s="4"/>
@@ -1369,16 +1404,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H34" s="1" t="str">
+      <c r="H34" s="1" t="e">
         <f t="shared" ref="H34:H64" si="4">IF(AND(G34&lt;&gt;" ",G34&lt;&gt;"ERROR",H33&lt;&gt;" ", H33&lt;&gt;"ERROR"),G34+H33," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I34" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
       <c r="D35" s="4"/>
@@ -1387,16 +1422,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H35" s="1" t="str">
+      <c r="H35" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I35" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="4"/>
@@ -1405,16 +1440,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H36" s="1" t="str">
+      <c r="H36" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I36" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
       <c r="D37" s="4"/>
@@ -1423,16 +1458,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H37" s="1" t="str">
+      <c r="H37" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I37" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
       <c r="D38" s="4"/>
@@ -1441,16 +1476,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H38" s="1" t="str">
+      <c r="H38" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I38" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="4"/>
@@ -1459,16 +1494,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H39" s="1" t="str">
+      <c r="H39" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I39" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
       <c r="D40" s="4"/>
@@ -1477,16 +1512,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H40" s="1" t="str">
+      <c r="H40" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I40" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="4"/>
@@ -1495,16 +1530,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H41" s="1" t="str">
+      <c r="H41" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I41" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:9">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
       <c r="D42" s="4"/>
@@ -1513,16 +1548,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H42" s="1" t="str">
+      <c r="H42" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I42" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:9">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
       <c r="D43" s="4"/>
@@ -1531,16 +1566,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H43" s="1" t="str">
+      <c r="H43" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I43" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:9">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="4"/>
       <c r="C44" s="5"/>
       <c r="D44" s="4"/>
@@ -1549,16 +1584,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H44" s="1" t="str">
+      <c r="H44" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I44" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:9">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="4"/>
       <c r="C45" s="5"/>
       <c r="D45" s="4"/>
@@ -1567,16 +1602,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H45" s="1" t="str">
+      <c r="H45" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I45" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:9">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" s="4"/>
       <c r="C46" s="5"/>
       <c r="D46" s="4"/>
@@ -1585,16 +1620,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H46" s="1" t="str">
+      <c r="H46" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I46" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:9">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" s="4"/>
       <c r="C47" s="5"/>
       <c r="D47" s="4"/>
@@ -1603,16 +1638,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H47" s="1" t="str">
+      <c r="H47" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I47" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:9">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" s="4"/>
       <c r="C48" s="5"/>
       <c r="D48" s="4"/>
@@ -1621,16 +1656,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H48" s="1" t="str">
+      <c r="H48" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I48" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:9">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
       <c r="D49" s="4"/>
@@ -1639,16 +1674,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H49" s="1" t="str">
+      <c r="H49" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I49" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="4"/>
       <c r="C50" s="5"/>
       <c r="D50" s="4"/>
@@ -1657,16 +1692,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H50" s="1" t="str">
+      <c r="H50" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I50" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" s="4"/>
       <c r="C51" s="5"/>
       <c r="D51" s="4"/>
@@ -1675,16 +1710,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H51" s="1" t="str">
+      <c r="H51" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I51" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" s="4"/>
       <c r="C52" s="5"/>
       <c r="D52" s="4"/>
@@ -1693,16 +1728,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H52" s="1" t="str">
+      <c r="H52" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I52" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" s="4"/>
       <c r="C53" s="5"/>
       <c r="D53" s="4"/>
@@ -1711,16 +1746,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H53" s="1" t="str">
+      <c r="H53" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I53" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" s="4"/>
       <c r="C54" s="5"/>
       <c r="D54" s="4"/>
@@ -1729,16 +1764,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H54" s="1" t="str">
+      <c r="H54" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I54" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="4"/>
       <c r="C55" s="5"/>
       <c r="D55" s="4"/>
@@ -1747,16 +1782,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H55" s="1" t="str">
+      <c r="H55" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I55" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" s="4"/>
       <c r="C56" s="5"/>
       <c r="D56" s="4"/>
@@ -1765,16 +1800,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H56" s="1" t="str">
+      <c r="H56" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I56" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:9">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" s="4"/>
       <c r="C57" s="5"/>
       <c r="D57" s="4"/>
@@ -1783,16 +1818,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H57" s="1" t="str">
+      <c r="H57" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I57" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:9">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58" s="4"/>
       <c r="C58" s="5"/>
       <c r="D58" s="4"/>
@@ -1801,16 +1836,16 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H58" s="1" t="str">
+      <c r="H58" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I58" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:9">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59" s="4"/>
       <c r="C59" s="5"/>
       <c r="D59" s="4"/>
@@ -1819,109 +1854,109 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H59" s="1" t="str">
+      <c r="H59" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I59" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:9">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60" s="4"/>
       <c r="G60" s="6" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H60" s="1" t="str">
+      <c r="H60" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I60" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:9">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" s="4"/>
       <c r="G61" s="6" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H61" s="1" t="str">
+      <c r="H61" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I61" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:9">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" s="4"/>
       <c r="G62" s="6" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H62" s="1" t="str">
+      <c r="H62" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I62" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:9">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" s="4"/>
       <c r="G63" s="6" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H63" s="1" t="str">
+      <c r="H63" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I63" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:9">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64" s="4"/>
       <c r="G64" s="6" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H64" s="1" t="str">
+      <c r="H64" s="1" t="e">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I64" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="16">
-      <c r="A65" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B65" s="9" t="s">
+    <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.4">
+      <c r="A65" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="10"/>
-      <c r="D65" s="9" t="s">
+      <c r="C65" s="16"/>
+      <c r="D65" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E65" s="10"/>
-      <c r="F65" s="11" t="s">
+      <c r="E65" s="16"/>
+      <c r="F65" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G65" s="11" t="s">
+      <c r="G65" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H65" s="11" t="s">
+      <c r="H65" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I65" s="1" t="e">
@@ -1929,8 +1964,8 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="16">
-      <c r="A66" s="8"/>
+    <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.4">
+      <c r="A66" s="9"/>
       <c r="B66" s="2" t="s">
         <v>2</v>
       </c>
@@ -1943,481 +1978,481 @@
       <c r="E66" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
       <c r="I66" s="1" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G67" s="6" t="str">
         <f t="shared" ref="G67:G98" si="5">IF(I67&gt;0,I67,IF(I67=0, " ", "ERROR"))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H67" s="1" t="str">
+      <c r="H67" s="1" t="e">
         <f>IF(AND(G67&lt;&gt;" ",G67&lt;&gt;"ERROR",H64&lt;&gt;" ", H64&lt;&gt;"ERROR"),G67+H64," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I67" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G68" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H68" s="1" t="str">
+      <c r="H68" s="1" t="e">
         <f t="shared" ref="H68:H98" si="6">IF(AND(G68&lt;&gt;" ",G68&lt;&gt;"ERROR",H67&lt;&gt;" ", H67&lt;&gt;"ERROR"),G68+H67," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I68" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G69" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H69" s="1" t="str">
+      <c r="H69" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I69" s="1">
         <f t="shared" ref="I69:I132" si="7">((D69+E69)-(B69+C69))*24</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G70" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H70" s="1" t="str">
+      <c r="H70" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I70" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G71" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H71" s="1" t="str">
+      <c r="H71" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I71" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G72" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H72" s="1" t="str">
+      <c r="H72" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I72" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G73" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H73" s="1" t="str">
+      <c r="H73" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I73" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G74" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H74" s="1" t="str">
+      <c r="H74" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I74" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G75" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H75" s="1" t="str">
+      <c r="H75" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I75" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G76" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H76" s="1" t="str">
+      <c r="H76" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I76" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G77" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H77" s="1" t="str">
+      <c r="H77" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I77" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G78" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H78" s="1" t="str">
+      <c r="H78" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I78" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G79" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H79" s="1" t="str">
+      <c r="H79" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I79" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G80" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H80" s="1" t="str">
+      <c r="H80" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I80" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="7:9">
+    <row r="81" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G81" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H81" s="1" t="str">
+      <c r="H81" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I81" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="7:9">
+    <row r="82" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G82" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H82" s="1" t="str">
+      <c r="H82" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I82" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="7:9">
+    <row r="83" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G83" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H83" s="1" t="str">
+      <c r="H83" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I83" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="7:9">
+    <row r="84" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G84" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H84" s="1" t="str">
+      <c r="H84" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I84" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="7:9">
+    <row r="85" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G85" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H85" s="1" t="str">
+      <c r="H85" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I85" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="7:9">
+    <row r="86" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G86" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H86" s="1" t="str">
+      <c r="H86" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I86" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="7:9">
+    <row r="87" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G87" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H87" s="1" t="str">
+      <c r="H87" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I87" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="7:9">
+    <row r="88" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G88" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H88" s="1" t="str">
+      <c r="H88" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I88" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="7:9">
+    <row r="89" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G89" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H89" s="1" t="str">
+      <c r="H89" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I89" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="7:9">
+    <row r="90" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G90" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H90" s="1" t="str">
+      <c r="H90" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I90" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="7:9">
+    <row r="91" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G91" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H91" s="1" t="str">
+      <c r="H91" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I91" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="7:9">
+    <row r="92" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G92" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H92" s="1" t="str">
+      <c r="H92" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I92" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="7:9">
+    <row r="93" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G93" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H93" s="1" t="str">
+      <c r="H93" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I93" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="7:9">
+    <row r="94" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G94" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H94" s="1" t="str">
+      <c r="H94" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I94" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="7:9">
+    <row r="95" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G95" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H95" s="1" t="str">
+      <c r="H95" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I95" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="7:9">
+    <row r="96" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G96" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H96" s="1" t="str">
+      <c r="H96" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I96" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G97" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H97" s="1" t="str">
+      <c r="H97" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I97" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G98" s="6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H98" s="1" t="str">
+      <c r="H98" s="1" t="e">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I98" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="16">
-      <c r="A99" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B99" s="9" t="s">
+    <row r="99" spans="1:9" ht="15" x14ac:dyDescent="0.4">
+      <c r="A99" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C99" s="10"/>
-      <c r="D99" s="9" t="s">
+      <c r="C99" s="16"/>
+      <c r="D99" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E99" s="10"/>
-      <c r="F99" s="11" t="s">
+      <c r="E99" s="16"/>
+      <c r="F99" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G99" s="11" t="s">
+      <c r="G99" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H99" s="11" t="s">
+      <c r="H99" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I99" s="1" t="e">
@@ -2425,8 +2460,8 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="16">
-      <c r="A100" s="8"/>
+    <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.4">
+      <c r="A100" s="9"/>
       <c r="B100" s="2" t="s">
         <v>2</v>
       </c>
@@ -2439,456 +2474,456 @@
       <c r="E100" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F100" s="11"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="11"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="7"/>
+      <c r="H100" s="7"/>
       <c r="I100" s="1" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G101" s="6" t="str">
         <f t="shared" ref="G101:G132" si="8">IF(I101&gt;0,I101,IF(I101=0, " ", "ERROR"))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H101" s="1" t="str">
+      <c r="H101" s="1" t="e">
         <f>IF(AND(G101&lt;&gt;" ",G101&lt;&gt;"ERROR",H98&lt;&gt;" ", H98&lt;&gt;"ERROR"),G101+H98," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I101" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G102" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H102" s="1" t="str">
+      <c r="H102" s="1" t="e">
         <f t="shared" ref="H102:H132" si="9">IF(AND(G102&lt;&gt;" ",G102&lt;&gt;"ERROR",H101&lt;&gt;" ", H101&lt;&gt;"ERROR"),G102+H101," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I102" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G103" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H103" s="1" t="str">
+      <c r="H103" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I103" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G104" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H104" s="1" t="str">
+      <c r="H104" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I104" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G105" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H105" s="1" t="str">
+      <c r="H105" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I105" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G106" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H106" s="1" t="str">
+      <c r="H106" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I106" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G107" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H107" s="1" t="str">
+      <c r="H107" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I107" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G108" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H108" s="1" t="str">
+      <c r="H108" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I108" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G109" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H109" s="1" t="str">
+      <c r="H109" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I109" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G110" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H110" s="1" t="str">
+      <c r="H110" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I110" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G111" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H111" s="1" t="str">
+      <c r="H111" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I111" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G112" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H112" s="1" t="str">
+      <c r="H112" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I112" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="7:9">
+    <row r="113" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G113" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H113" s="1" t="str">
+      <c r="H113" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I113" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="7:9">
+    <row r="114" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G114" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H114" s="1" t="str">
+      <c r="H114" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I114" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="7:9">
+    <row r="115" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G115" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H115" s="1" t="str">
+      <c r="H115" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I115" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="7:9">
+    <row r="116" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G116" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H116" s="1" t="str">
+      <c r="H116" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I116" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="7:9">
+    <row r="117" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G117" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H117" s="1" t="str">
+      <c r="H117" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I117" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="7:9">
+    <row r="118" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G118" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H118" s="1" t="str">
+      <c r="H118" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I118" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="7:9">
+    <row r="119" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G119" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H119" s="1" t="str">
+      <c r="H119" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I119" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="7:9">
+    <row r="120" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G120" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H120" s="1" t="str">
+      <c r="H120" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I120" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="7:9">
+    <row r="121" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G121" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H121" s="1" t="str">
+      <c r="H121" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I121" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="7:9">
+    <row r="122" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G122" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H122" s="1" t="str">
+      <c r="H122" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I122" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="7:9">
+    <row r="123" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G123" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H123" s="1" t="str">
+      <c r="H123" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I123" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="7:9">
+    <row r="124" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G124" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H124" s="1" t="str">
+      <c r="H124" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I124" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="7:9">
+    <row r="125" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G125" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H125" s="1" t="str">
+      <c r="H125" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I125" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="7:9">
+    <row r="126" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G126" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H126" s="1" t="str">
+      <c r="H126" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I126" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="7:9">
+    <row r="127" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G127" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H127" s="1" t="str">
+      <c r="H127" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I127" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="7:9">
+    <row r="128" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G128" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H128" s="1" t="str">
+      <c r="H128" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I128" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="7:9">
+    <row r="129" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G129" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H129" s="1" t="str">
+      <c r="H129" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I129" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="7:9">
+    <row r="130" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G130" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H130" s="1" t="str">
+      <c r="H130" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I130" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="7:9">
+    <row r="131" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G131" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H131" s="1" t="str">
+      <c r="H131" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I131" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="7:9">
+    <row r="132" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G132" s="6" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H132" s="1" t="str">
+      <c r="H132" s="1" t="e">
         <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
+        <v>#VALUE!</v>
       </c>
       <c r="I132" s="1">
         <f t="shared" si="7"/>
@@ -2897,6 +2932,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="H99:H100"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="F99:F100"/>
+    <mergeCell ref="G99:G100"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="H65:H66"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:F66"/>
     <mergeCell ref="H31:H32"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A1:H1"/>
@@ -2909,19 +2956,7 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:F66"/>
     <mergeCell ref="G31:G32"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="F99:F100"/>
-    <mergeCell ref="G99:G100"/>
-    <mergeCell ref="H99:H100"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -2931,12 +2966,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2946,12 +2981,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>